<commit_message>
HuyBD: Update Report.docx, ListAction.xlsx
</commit_message>
<xml_diff>
--- a/Temp/ListAction.xlsx
+++ b/Temp/ListAction.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FTS\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FTS\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Owner</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>Huy: design generate report (create, review); core module</t>
+  </si>
+  <si>
+    <t>Thien: mobile app for truck driver, design UI, find CSS template, web services for mobile app</t>
+  </si>
+  <si>
+    <t>Thinh: mobile app for goods owner, web services for mobile app</t>
+  </si>
+  <si>
+    <t>Khuong: web app, webservice for web</t>
   </si>
 </sst>
 </file>
@@ -185,6 +197,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -192,15 +213,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,19 +494,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -502,88 +515,100 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>